<commit_message>
BACKTEST working as well.
</commit_message>
<xml_diff>
--- a/sst.xlsx
+++ b/sst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\12. Rohit POC\5. binance\4. stock market\sst_stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85319B35-E65B-4F70-952C-05D21C4E9D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0290AA86-950A-4C4E-A338-D5DAA82F64CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="125">
   <si>
     <t>SYMBOL</t>
   </si>
@@ -828,7 +828,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A99"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4004,10 +4006,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4022,22 +4024,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BackTeating code working correctly
</commit_message>
<xml_diff>
--- a/sst.xlsx
+++ b/sst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\12. Rohit POC\5. binance\4. stock market\sst_stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0290AA86-950A-4C4E-A338-D5DAA82F64CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA627B0-65BB-4ADD-92C2-8406B706F970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -828,7 +828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A99"/>
     </sheetView>
   </sheetViews>
@@ -3525,8 +3525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4024,7 +4024,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>